<commit_message>
closer, still need route param to work
</commit_message>
<xml_diff>
--- a/include/genstrings.xlsx
+++ b/include/genstrings.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="82">
   <si>
     <t>// person info</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,14 +603,15 @@
     <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -628,11 +632,15 @@
         <v>s</v>
       </c>
       <c r="F2" t="str">
-        <f>E2&amp;F1</f>
-        <v>s</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <f>E2</f>
+        <v>s</v>
+      </c>
+      <c r="G2" t="str">
+        <f xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A2)&amp;", TRUE ));"</f>
+        <v>error_log( print_R($LastName, TRUE ));</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -653,11 +661,15 @@
         <v>s</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F34" si="3">E3&amp;F2</f>
+        <f>F2&amp;E3</f>
         <v>ss</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G33" si="3" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A3)&amp;", TRUE ));"</f>
+        <v>error_log( print_R($FirstName, TRUE ));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -678,11 +690,15 @@
         <v>s</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F4:F34" si="4">F3&amp;E4</f>
         <v>sss</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Email, TRUE ));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -703,11 +719,15 @@
         <v>s</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssss</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Email2, TRUE ));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -728,11 +748,15 @@
         <v>s</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssss</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Phone, TRUE ));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -753,11 +777,15 @@
         <v>s</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssss</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($AltPhone, TRUE ));</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -778,11 +806,15 @@
         <v>s</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssss</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($phoneExt, TRUE ));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -803,11 +835,15 @@
         <v>s</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssss</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($altPhoneExt, TRUE ));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -828,11 +864,15 @@
         <v>s</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssss</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Birthday, TRUE ));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -853,11 +893,15 @@
         <v>s</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssss</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($sex, TRUE ));</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -878,11 +922,15 @@
         <v>s</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssss</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Parent, TRUE ));</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -903,11 +951,15 @@
         <v>s</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssss</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($EmergencyContact, TRUE ));</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -928,11 +980,15 @@
         <v>s</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssss</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Notes, TRUE ));</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -953,11 +1009,15 @@
         <v>s</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssssss</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($medicalConcerns, TRUE ));</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -978,11 +1038,15 @@
         <v>s</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssssss</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($Address, TRUE ));</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1003,11 +1067,15 @@
         <v>s</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssssssss</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($City, TRUE ));</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1028,11 +1096,15 @@
         <v>s</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssssssss</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($State, TRUE ));</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1053,11 +1125,15 @@
         <v>s</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($ZIP, TRUE ));</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1078,11 +1154,15 @@
         <v>s</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($ContactType, TRUE ));</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1103,11 +1183,15 @@
         <v>s</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($quickbooklink, TRUE ));</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1128,11 +1212,15 @@
         <v>s</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($StudentSchool, TRUE ));</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1153,11 +1241,15 @@
         <v>s</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ssssssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($GuiSize, TRUE ));</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1178,11 +1270,15 @@
         <v>s</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>sssssssssssssssssssssss</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($ShirtSize, TRUE ));</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1203,11 +1299,15 @@
         <v>d</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="3"/>
-        <v>dsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssd</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($BeltSize, TRUE ));</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1228,11 +1328,15 @@
         <v>s</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="3"/>
-        <v>sdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssds</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($ReferredBy, TRUE ));</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1250,14 +1354,18 @@
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(A27,Sheet2!B:I,8,FALSE)</f>
-        <v>i</v>
+        <v>x</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="3"/>
-        <v>isdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsx</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($InstructorPaymentFree, TRUE ));</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1275,14 +1383,18 @@
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(A28,Sheet2!B:I,8,FALSE)</f>
-        <v>i</v>
+        <v>x</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="3"/>
-        <v>iisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxx</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($InstructorFlag, TRUE ));</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1303,11 +1415,15 @@
         <v>s</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="3"/>
-        <v>siisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxs</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($instructorTitle, TRUE ));</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1328,11 +1444,15 @@
         <v>s</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="3"/>
-        <v>ssiisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxss</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($CurrentRank, TRUE ));</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1353,11 +1473,15 @@
         <v>s</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="3"/>
-        <v>sssiisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxsss</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($CurrentReikiRank, TRUE ));</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1378,16 +1502,20 @@
         <v>s</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="3"/>
-        <v>ssssiisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxssss</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($CurrentIARank, TRUE ));</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" ref="B3:B33" si="4">"$sql .= """&amp;" t."&amp;TRIM(A33)&amp;" = :"&amp;TRIM(A33)&amp;", "&amp;""";"</f>
+        <f t="shared" ref="B33" si="5">"$sql .= """&amp;" t."&amp;TRIM(A33)&amp;" = :"&amp;TRIM(A33)&amp;", "&amp;""";"</f>
         <v>$sql .= " t.ID = :ID, ";</v>
       </c>
       <c r="C33" t="str">
@@ -1403,14 +1531,18 @@
         <v>i</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="3"/>
-        <v>issssiisdsssssssssssssssssssssss</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxssssi</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>error_log( print_R($ID, TRUE ));</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" t="str">
-        <f t="shared" si="3"/>
-        <v>issssiisdsssssssssssssssssssssss</v>
+        <f t="shared" si="4"/>
+        <v>sssssssssssssssssssssssdsxxssssi</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
@@ -1901,7 +2033,7 @@
         <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1938,7 +2070,7 @@
         <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1981,7 +2113,7 @@
         <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1998,7 +2130,7 @@
         <v>17</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -2119,7 +2251,7 @@
         <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -2381,7 +2513,7 @@
         <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
student lists filling the dojo portion of student
</commit_message>
<xml_diff>
--- a/include/genstrings.xlsx
+++ b/include/genstrings.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="74">
   <si>
     <t>// person info</t>
   </si>
@@ -84,9 +84,6 @@
     <t>b'0',</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>'Student',</t>
   </si>
   <si>
@@ -168,15 +165,6 @@
     <t>LastPromoted</t>
   </si>
   <si>
-    <t>ReferredBy</t>
-  </si>
-  <si>
-    <t>ConsentToPublicPictures</t>
-  </si>
-  <si>
-    <t>Attachments</t>
-  </si>
-  <si>
     <t>InstructorPaymentFree</t>
   </si>
   <si>
@@ -204,9 +192,6 @@
     <t>bdayinclude</t>
   </si>
   <si>
-    <t>signupDate</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -232,15 +217,6 @@
   </si>
   <si>
     <t>EmergencyContact</t>
-  </si>
-  <si>
-    <t>sendWelcomeCard</t>
-  </si>
-  <si>
-    <t>dateEntered</t>
-  </si>
-  <si>
-    <t>dateInactive</t>
   </si>
   <si>
     <t>CurrentIARank</t>
@@ -591,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G33"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +589,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="str">
         <f>"$sql .= """&amp;" t."&amp;TRIM(A2)&amp;" = ?," &amp;""";"</f>
@@ -642,18 +618,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B32" si="0">"$sql .= """&amp;" t."&amp;TRIM(A3)&amp;" = ?," &amp;""";"</f>
+        <f t="shared" ref="B3:B31" si="0">"$sql .= """&amp;" t."&amp;TRIM(A3)&amp;" = ?," &amp;""";"</f>
         <v>$sql .= " t.FirstName = ?,";</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C33" si="1">"$student-&gt;"&amp;TRIM(A3)&amp;","</f>
+        <f t="shared" ref="C3:C32" si="1">"$student-&gt;"&amp;TRIM(A3)&amp;","</f>
         <v>$student-&gt;FirstName,</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D33" si="2">"$"&amp;TRIM(A3)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A3)&amp;"');"</f>
+        <f t="shared" ref="D3:D32" si="2">"$"&amp;TRIM(A3)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A3)&amp;"');"</f>
         <v>$FirstName = $app-&gt;request-&gt;put('FirstName');</v>
       </c>
       <c r="E3" t="str">
@@ -665,13 +641,13 @@
         <v>ss</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G33" si="3" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A3)&amp;", TRUE ));"</f>
+        <f t="shared" ref="G3:G32" si="3" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A3)&amp;", TRUE ));"</f>
         <v>error_log( print_R($FirstName, TRUE ));</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -690,7 +666,7 @@
         <v>s</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F34" si="4">F3&amp;E4</f>
+        <f t="shared" ref="F4:F33" si="4">F3&amp;E4</f>
         <v>sss</v>
       </c>
       <c r="G4" t="str">
@@ -700,7 +676,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -729,7 +705,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -758,7 +734,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -787,7 +763,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -816,7 +792,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -845,7 +821,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -874,7 +850,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -903,7 +879,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -932,7 +908,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -961,7 +937,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -990,7 +966,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -1019,7 +995,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -1048,7 +1024,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -1077,7 +1053,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -1106,7 +1082,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -1135,7 +1111,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -1164,7 +1140,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -1193,7 +1169,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -1222,7 +1198,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -1251,7 +1227,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -1280,7 +1256,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -1309,48 +1285,48 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.ReferredBy = ?,";</v>
+        <v>$sql .= " t.InstructorPaymentFree = ?,";</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;ReferredBy,</v>
+        <v>$student-&gt;InstructorPaymentFree,</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="2"/>
-        <v>$ReferredBy = $app-&gt;request-&gt;put('ReferredBy');</v>
+        <v>$InstructorPaymentFree = $app-&gt;request-&gt;put('InstructorPaymentFree');</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(A26,Sheet2!B:I,8,FALSE)</f>
-        <v>s</v>
+        <v>x</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssds</v>
+        <v>sssssssssssssssssssssssdx</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($ReferredBy, TRUE ));</v>
+        <v>error_log( print_R($InstructorPaymentFree, TRUE ));</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.InstructorPaymentFree = ?,";</v>
+        <v>$sql .= " t.InstructorFlag = ?,";</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;InstructorPaymentFree,</v>
+        <v>$student-&gt;InstructorFlag,</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
-        <v>$InstructorPaymentFree = $app-&gt;request-&gt;put('InstructorPaymentFree');</v>
+        <v>$InstructorFlag = $app-&gt;request-&gt;put('InstructorFlag');</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(A27,Sheet2!B:I,8,FALSE)</f>
@@ -1358,57 +1334,57 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsx</v>
+        <v>sssssssssssssssssssssssdxx</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($InstructorPaymentFree, TRUE ));</v>
+        <v>error_log( print_R($InstructorFlag, TRUE ));</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.InstructorFlag = ?,";</v>
+        <v>$sql .= " t.instructorTitle = ?,";</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;InstructorFlag,</v>
+        <v>$student-&gt;instructorTitle,</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
-        <v>$InstructorFlag = $app-&gt;request-&gt;put('InstructorFlag');</v>
+        <v>$instructorTitle = $app-&gt;request-&gt;put('instructorTitle');</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(A28,Sheet2!B:I,8,FALSE)</f>
-        <v>x</v>
+        <v>s</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxx</v>
+        <v>sssssssssssssssssssssssdxxs</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($InstructorFlag, TRUE ));</v>
+        <v>error_log( print_R($instructorTitle, TRUE ));</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.instructorTitle = ?,";</v>
+        <v>$sql .= " t.CurrentRank = ?,";</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;instructorTitle,</v>
+        <v>$student-&gt;CurrentRank,</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="2"/>
-        <v>$instructorTitle = $app-&gt;request-&gt;put('instructorTitle');</v>
+        <v>$CurrentRank = $app-&gt;request-&gt;put('CurrentRank');</v>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(A29,Sheet2!B:I,8,FALSE)</f>
@@ -1416,28 +1392,28 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxs</v>
+        <v>sssssssssssssssssssssssdxxss</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($instructorTitle, TRUE ));</v>
+        <v>error_log( print_R($CurrentRank, TRUE ));</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.CurrentRank = ?,";</v>
+        <v>$sql .= " t.CurrentReikiRank = ?,";</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;CurrentRank,</v>
+        <v>$student-&gt;CurrentReikiRank,</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="2"/>
-        <v>$CurrentRank = $app-&gt;request-&gt;put('CurrentRank');</v>
+        <v>$CurrentReikiRank = $app-&gt;request-&gt;put('CurrentReikiRank');</v>
       </c>
       <c r="E30" t="str">
         <f>VLOOKUP(A30,Sheet2!B:I,8,FALSE)</f>
@@ -1445,28 +1421,28 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxss</v>
+        <v>sssssssssssssssssssssssdxxsss</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($CurrentRank, TRUE ));</v>
+        <v>error_log( print_R($CurrentReikiRank, TRUE ));</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>$sql .= " t.CurrentReikiRank = ?,";</v>
+        <v>$sql .= " t.CurrentIARank = ?,";</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;CurrentReikiRank,</v>
+        <v>$student-&gt;CurrentIARank,</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="2"/>
-        <v>$CurrentReikiRank = $app-&gt;request-&gt;put('CurrentReikiRank');</v>
+        <v>$CurrentIARank = $app-&gt;request-&gt;put('CurrentIARank');</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(A31,Sheet2!B:I,8,FALSE)</f>
@@ -1474,75 +1450,46 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxsss</v>
+        <v>sssssssssssssssssssssssdxxssss</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($CurrentReikiRank, TRUE ));</v>
+        <v>error_log( print_R($CurrentIARank, TRUE ));</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>$sql .= " t.CurrentIARank = ?,";</v>
+        <f t="shared" ref="B32" si="5">"$sql .= """&amp;" t."&amp;TRIM(A32)&amp;" = :"&amp;TRIM(A32)&amp;", "&amp;""";"</f>
+        <v>$sql .= " t.ID = :ID, ";</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
-        <v>$student-&gt;CurrentIARank,</v>
+        <v>$student-&gt;ID,</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="2"/>
-        <v>$CurrentIARank = $app-&gt;request-&gt;put('CurrentIARank');</v>
+        <v>$ID = $app-&gt;request-&gt;put('ID');</v>
       </c>
       <c r="E32" t="str">
         <f>VLOOKUP(A32,Sheet2!B:I,8,FALSE)</f>
-        <v>s</v>
+        <v>i</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxssss</v>
+        <v>sssssssssssssssssssssssdxxssssi</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="3"/>
-        <v>error_log( print_R($CurrentIARank, TRUE ));</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" ref="B33" si="5">"$sql .= """&amp;" t."&amp;TRIM(A33)&amp;" = :"&amp;TRIM(A33)&amp;", "&amp;""";"</f>
-        <v>$sql .= " t.ID = :ID, ";</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="1"/>
-        <v>$student-&gt;ID,</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="2"/>
-        <v>$ID = $app-&gt;request-&gt;put('ID');</v>
-      </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(A33,Sheet2!B:I,8,FALSE)</f>
-        <v>i</v>
-      </c>
+        <v>error_log( print_R($ID, TRUE ));</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxssssi</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="3"/>
-        <v>error_log( print_R($ID, TRUE ));</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F34" t="str">
-        <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdsxxssssi</v>
+        <v>sssssssssssssssssssssssdxxssssi</v>
       </c>
     </row>
   </sheetData>
@@ -1553,11 +1500,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I49"/>
+  <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1569,7 +1514,7 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1590,12 +1535,12 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1616,12 +1561,12 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1642,12 +1587,12 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1668,12 +1613,12 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1694,12 +1639,12 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1720,12 +1665,12 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1746,12 +1691,12 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1772,12 +1717,12 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -1798,12 +1743,12 @@
         <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1824,12 +1769,12 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1850,12 +1795,12 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1870,12 +1815,12 @@
         <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1887,12 +1832,12 @@
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1904,12 +1849,12 @@
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1930,12 +1875,12 @@
         <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1947,12 +1892,12 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1973,12 +1918,12 @@
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1990,75 +1935,72 @@
         <v>6</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -2070,12 +2012,12 @@
         <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -2093,49 +2035,67 @@
         <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
       </c>
       <c r="I24" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -2156,38 +2116,29 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -2205,18 +2156,18 @@
         <v>5</v>
       </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -2225,55 +2176,67 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I29" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>21</v>
       </c>
       <c r="I31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -2291,18 +2254,18 @@
         <v>5</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>
@@ -2311,15 +2274,21 @@
         <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" t="s">
+        <v>6</v>
       </c>
       <c r="I33" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -2337,15 +2306,15 @@
         <v>5</v>
       </c>
       <c r="H34" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -2363,15 +2332,15 @@
         <v>5</v>
       </c>
       <c r="H35" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I35" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -2392,12 +2361,12 @@
         <v>6</v>
       </c>
       <c r="I36" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -2418,41 +2387,32 @@
         <v>6</v>
       </c>
       <c r="I37" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
@@ -2470,204 +2430,58 @@
         <v>6</v>
       </c>
       <c r="I39" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I40" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
       </c>
       <c r="I42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
         <v>70</v>
-      </c>
-      <c r="C43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" t="s">
-        <v>6</v>
-      </c>
-      <c r="I43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
-        <v>4</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" t="s">
-        <v>4</v>
-      </c>
-      <c r="G46" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>6</v>
-      </c>
-      <c r="I46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-      <c r="I48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" t="s">
-        <v>6</v>
-      </c>
-      <c r="I49" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checkbox and instructor payment added
</commit_message>
<xml_diff>
--- a/include/genstrings.xlsx
+++ b/include/genstrings.xlsx
@@ -1301,11 +1301,11 @@
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(A26,Sheet2!B:I,8,FALSE)</f>
-        <v>x</v>
+        <v>i</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdx</v>
+        <v>sssssssssssssssssssssssdi</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="3"/>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxx</v>
+        <v>sssssssssssssssssssssssdix</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="3"/>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxs</v>
+        <v>sssssssssssssssssssssssdixs</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="3"/>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxss</v>
+        <v>sssssssssssssssssssssssdixss</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="3"/>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxsss</v>
+        <v>sssssssssssssssssssssssdixsss</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="3"/>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxssss</v>
+        <v>sssssssssssssssssssssssdixssss</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="3"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxssssi</v>
+        <v>sssssssssssssssssssssssdixssssi</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="3"/>
@@ -1489,7 +1489,7 @@
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" t="str">
         <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdxxssssi</v>
+        <v>sssssssssssssssssssssssdixssssi</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1943,16 +1945,16 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
beginning of model for student class
</commit_message>
<xml_diff>
--- a/include/genstrings.xlsx
+++ b/include/genstrings.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="92">
   <si>
     <t>// person info</t>
   </si>
@@ -250,6 +251,60 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>contactid</t>
+  </si>
+  <si>
+    <t>classid</t>
+  </si>
+  <si>
+    <t>classPayName</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>altPhone</t>
+  </si>
+  <si>
+    <t>isTestFeeWaived</t>
+  </si>
+  <si>
+    <t>autoBillEFTDate</t>
+  </si>
+  <si>
+    <t>firstPaymentDate</t>
+  </si>
+  <si>
+    <t>ncontacts</t>
+  </si>
+  <si>
+    <t>nclasspays</t>
+  </si>
+  <si>
+    <t>//nclasspays</t>
+  </si>
+  <si>
+    <t>int(1)</t>
+  </si>
+  <si>
+    <t>contactID</t>
   </si>
 </sst>
 </file>
@@ -567,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +721,7 @@
         <v>s</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F33" si="4">F3&amp;E4</f>
+        <f t="shared" ref="F4:F32" si="4">F3&amp;E4</f>
         <v>sss</v>
       </c>
       <c r="G4" t="str">
@@ -1486,10 +1541,154 @@
         <v>error_log( print_R($ID, TRUE ));</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" t="str">
-        <f t="shared" si="4"/>
-        <v>sssssssssssssssssssssssdixssssi</v>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ref="B35:B36" si="6">"$sql .= """&amp;" t."&amp;TRIM(A35)&amp;" = :"&amp;TRIM(A35)&amp;", "&amp;""";"</f>
+        <v>$sql .= " t.contactID = :contactID, ";</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ref="C35:C36" si="7">"$student-&gt;"&amp;TRIM(A35)&amp;","</f>
+        <v>$student-&gt;contactID,</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35:D36" si="8">"$"&amp;TRIM(A35)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A35)&amp;"');"</f>
+        <v>$contactID = $app-&gt;request-&gt;put('contactID');</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP(A35,Sheet3!B:I,8,FALSE)</f>
+        <v>i</v>
+      </c>
+      <c r="F35" t="str">
+        <f>E35</f>
+        <v>i</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" ref="G35:G36" si="9" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A35)&amp;", TRUE ));"</f>
+        <v>error_log( print_R($contactID, TRUE ));</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="6"/>
+        <v>$sql .= " t.classid = :classid, ";</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="7"/>
+        <v>$student-&gt;classid,</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="8"/>
+        <v>$classid = $app-&gt;request-&gt;put('classid');</v>
+      </c>
+      <c r="E36" t="str">
+        <f>VLOOKUP(A36,Sheet3!B:I,8,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" ref="F36" si="10">F35&amp;E36</f>
+        <v>is</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="9"/>
+        <v>error_log( print_R($classid, TRUE ));</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" ref="B36:B39" si="11">"$sql .= """&amp;" t."&amp;TRIM(A37)&amp;" = :"&amp;TRIM(A37)&amp;", "&amp;""";"</f>
+        <v>$sql .= " t.classPayName = :classPayName, ";</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" ref="C36:C39" si="12">"$student-&gt;"&amp;TRIM(A37)&amp;","</f>
+        <v>$student-&gt;classPayName,</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D36:D39" si="13">"$"&amp;TRIM(A37)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A37)&amp;"');"</f>
+        <v>$classPayName = $app-&gt;request-&gt;put('classPayName');</v>
+      </c>
+      <c r="E37" t="str">
+        <f>VLOOKUP(A37,Sheet3!B:I,8,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" ref="F37:F39" si="14">F36&amp;E37</f>
+        <v>iss</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" ref="G36:G39" si="15" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A37)&amp;", TRUE ));"</f>
+        <v>error_log( print_R($classPayName, TRUE ));</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="11"/>
+        <v>$sql .= " t.class = :class, ";</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="12"/>
+        <v>$student-&gt;class,</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="13"/>
+        <v>$class = $app-&gt;request-&gt;put('class');</v>
+      </c>
+      <c r="E38" t="str">
+        <f>VLOOKUP(A38,Sheet3!B:I,8,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="14"/>
+        <v>isss</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="15"/>
+        <v>error_log( print_R($class, TRUE ));</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="11"/>
+        <v>$sql .= " t.isTestFeeWaived = :isTestFeeWaived, ";</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="12"/>
+        <v>$student-&gt;isTestFeeWaived,</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="13"/>
+        <v>$isTestFeeWaived = $app-&gt;request-&gt;put('isTestFeeWaived');</v>
+      </c>
+      <c r="E39" t="str">
+        <f>VLOOKUP(A39,Sheet3!B:I,8,FALSE)</f>
+        <v>i</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="14"/>
+        <v>isssi</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="15"/>
+        <v>error_log( print_R($isTestFeeWaived, TRUE ));</v>
       </c>
     </row>
   </sheetData>
@@ -1500,10 +1699,436 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I42"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +2139,10 @@
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
       <c r="B1" t="s">
         <v>27</v>
       </c>
@@ -1540,7 +2168,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>28</v>
       </c>
@@ -1566,7 +2194,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -1592,7 +2220,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -1618,7 +2246,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -1644,7 +2272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -1670,7 +2298,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1696,7 +2324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1722,7 +2350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -1748,7 +2376,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -1774,7 +2402,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -1800,7 +2428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -1820,7 +2448,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -1837,7 +2465,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>40</v>
       </c>
@@ -1854,7 +2482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1880,7 +2508,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -2488,5 +3116,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
class status update working
</commit_message>
<xml_diff>
--- a/include/genstrings.xlsx
+++ b/include/genstrings.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="94">
   <si>
     <t>// person info</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>contactID</t>
+  </si>
+  <si>
+    <t>studentclassstatus</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35:K39"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1621,7 @@
         <v>$sql .= " t.classid = :classid, ";</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36:C39" si="9">"$studentclass-&gt;"&amp;TRIM(A36)&amp;","</f>
+        <f t="shared" ref="C36:C40" si="9">"$studentclass-&gt;"&amp;TRIM(A36)&amp;","</f>
         <v>$studentclass-&gt;classid,</v>
       </c>
       <c r="D36" t="str">
@@ -1635,27 +1641,27 @@
         <v>error_log( print_R($classid, TRUE ));</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f t="shared" ref="H36:H39" si="11">"$response["""&amp;TRIM(A36)&amp;"""] = $result["""&amp;TRIM(A36)&amp;"""];"</f>
+        <f t="shared" ref="H36:H40" si="11">"$response["""&amp;TRIM(A36)&amp;"""] = $result["""&amp;TRIM(A36)&amp;"""];"</f>
         <v>$response["classid"] = $result["classid"];</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" ref="I36:I39" si="12">"$"&amp;TRIM(A36)&amp;" = $studentclass-&gt;"&amp;TRIM(A36)&amp;";"</f>
+        <f t="shared" ref="I36:I40" si="12">"$"&amp;TRIM(A36)&amp;" = $studentclass-&gt;"&amp;TRIM(A36)&amp;";"</f>
         <v>$classid = $studentclass-&gt;classid;</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" ref="J36:J39" si="13">"$"&amp;TRIM(A36)&amp;","</f>
+        <f t="shared" ref="J36:J40" si="13">"$"&amp;TRIM(A36)&amp;","</f>
         <v>$classid,</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" ref="K36:K39" si="14">"$res[""sc_"&amp;TRIM(A36)&amp;"""] = $sc_"&amp;TRIM(A36)&amp;";"</f>
+        <f t="shared" ref="K36:K40" si="14">"$res[""sc_"&amp;TRIM(A36)&amp;"""] = $sc_"&amp;TRIM(A36)&amp;";"</f>
         <v>$res["sc_classid"] = $sc_classid;</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" ref="L36:L39" si="15">"t."&amp;TRIM(A36)&amp;","</f>
+        <f t="shared" ref="L36:L40" si="15">"t."&amp;TRIM(A36)&amp;","</f>
         <v>t.classid,</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" ref="M36:M39" si="16">"$sc_"&amp;TRIM(A36)&amp;","</f>
+        <f t="shared" ref="M36:M40" si="16">"$sc_"&amp;TRIM(A36)&amp;","</f>
         <v>$sc_classid,</v>
       </c>
     </row>
@@ -1664,7 +1670,7 @@
         <v>76</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" ref="B37:B39" si="17">"$sql .= """&amp;" t."&amp;TRIM(A37)&amp;" = :"&amp;TRIM(A37)&amp;", "&amp;""";"</f>
+        <f t="shared" ref="B37:B40" si="17">"$sql .= """&amp;" t."&amp;TRIM(A37)&amp;" = :"&amp;TRIM(A37)&amp;", "&amp;""";"</f>
         <v>$sql .= " t.classPayName = :classPayName, ";</v>
       </c>
       <c r="C37" t="str">
@@ -1672,7 +1678,7 @@
         <v>$studentclass-&gt;classPayName,</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" ref="D37:D39" si="18">"$"&amp;TRIM(A37)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A37)&amp;"');"</f>
+        <f t="shared" ref="D37:D40" si="18">"$"&amp;TRIM(A37)&amp;" = $app-&gt;request-&gt;put('"&amp;TRIM(A37)&amp;"');"</f>
         <v>$classPayName = $app-&gt;request-&gt;put('classPayName');</v>
       </c>
       <c r="E37" t="str">
@@ -1684,7 +1690,7 @@
         <v>iss</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" ref="G37:G39" si="20" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A37)&amp;", TRUE ));"</f>
+        <f t="shared" ref="G37:G40" si="20" xml:space="preserve"> "error_log( print_R($"&amp;TRIM(A37)&amp;", TRUE ));"</f>
         <v>error_log( print_R($classPayName, TRUE ));</v>
       </c>
       <c r="H37" s="1" t="str">
@@ -1816,6 +1822,59 @@
       <c r="M39" t="str">
         <f t="shared" si="16"/>
         <v>$sc_isTestFeeWaived,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="17"/>
+        <v>$sql .= " t.studentclassstatus = :studentclassstatus, ";</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="9"/>
+        <v>$studentclass-&gt;studentclassstatus,</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="18"/>
+        <v>$studentclassstatus = $app-&gt;request-&gt;put('studentclassstatus');</v>
+      </c>
+      <c r="E40" t="str">
+        <f>VLOOKUP(A40,Sheet3!B:I,8,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" ref="F40" si="21">F39&amp;E40</f>
+        <v>isssis</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="20"/>
+        <v>error_log( print_R($studentclassstatus, TRUE ));</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="11"/>
+        <v>$response["studentclassstatus"] = $result["studentclassstatus"];</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="12"/>
+        <v>$studentclassstatus = $studentclass-&gt;studentclassstatus;</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="13"/>
+        <v>$studentclassstatus,</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="14"/>
+        <v>$res["sc_studentclassstatus"] = $sc_studentclassstatus;</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="15"/>
+        <v>t.studentclassstatus,</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="16"/>
+        <v>$sc_studentclassstatus,</v>
       </c>
     </row>
   </sheetData>
@@ -1826,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,6 +2302,32 @@
       </c>
       <c r="I17" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>